<commit_message>
Commit Cy.2: MOD-01-TS-001_Elements_Text Box Design and Execution completed
</commit_message>
<xml_diff>
--- a/References/Hands-on Exercise/DemoQA-Test Design.xlsx
+++ b/References/Hands-on Exercise/DemoQA-Test Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1bf4b082bbe3/Desktop/Projects/Testing Projects/References/Hands-on Exercise/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F25DC773A252ABDACC1048CAE1D9486A5ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D144DB1D-A059-453F-8A27-994ADDB99F05}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC1048CAE1D9486A5ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E39FBDD-0D8C-49A2-97DB-AE769C9403A8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="338">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -1602,6 +1602,27 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>testdata-TS01.json</t>
+  </si>
+  <si>
+    <t>System didn't thrown error message. Some inputs It throws accepted</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>TC001-03</t>
+  </si>
+  <si>
+    <t>Validate text input submission at edge level</t>
+  </si>
+  <si>
+    <t>Details of the form input should not be displayed</t>
+  </si>
+  <si>
+    <t>Details of the form input are not be displayed</t>
   </si>
 </sst>
 </file>
@@ -3999,10 +4020,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A0535F-E9BA-4BD0-B898-820EEEB24304}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,18 +4031,18 @@
     <col min="1" max="1" width="15.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="95.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" style="10" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="10" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="161.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="93.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="146.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="49" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" style="10" customWidth="1"/>
     <col min="16" max="16" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="10" bestFit="1" customWidth="1"/>
@@ -4066,7 +4087,7 @@
       <c r="L1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="N1" s="6" t="s">
@@ -4088,7 +4109,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>109</v>
       </c>
@@ -4143,7 +4164,7 @@
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>109</v>
       </c>
@@ -4181,63 +4202,79 @@
         <v>257</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
+        <v>336</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>330</v>
+      </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>259</v>
+        <v>334</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>260</v>
+        <v>335</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="I4" s="7">
         <v>2</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
+        <v>258</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>333</v>
+      </c>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>110</v>
       </c>
@@ -4251,13 +4288,13 @@
         <v>139</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>54</v>
@@ -4266,16 +4303,16 @@
         <v>2</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>320</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
@@ -4284,45 +4321,45 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>54</v>
       </c>
       <c r="I6" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
@@ -4331,45 +4368,45 @@
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>54</v>
       </c>
       <c r="I7" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
@@ -4378,7 +4415,7 @@
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>112</v>
       </c>
@@ -4392,13 +4429,13 @@
         <v>141</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>54</v>
@@ -4407,16 +4444,16 @@
         <v>4</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>322</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -4425,7 +4462,7 @@
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>112</v>
       </c>
@@ -4439,13 +4476,13 @@
         <v>141</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>54</v>
@@ -4460,10 +4497,10 @@
         <v>322</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
@@ -4472,7 +4509,7 @@
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>112</v>
       </c>
@@ -4486,13 +4523,13 @@
         <v>141</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>54</v>
@@ -4507,10 +4544,10 @@
         <v>322</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -4519,45 +4556,45 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>54</v>
       </c>
       <c r="I11" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
@@ -4566,9 +4603,9 @@
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>52</v>
@@ -4580,13 +4617,13 @@
         <v>142</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>63</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>54</v>
@@ -4601,10 +4638,10 @@
         <v>323</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -4613,9 +4650,9 @@
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>52</v>
@@ -4627,13 +4664,13 @@
         <v>142</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>63</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>54</v>
@@ -4648,10 +4685,10 @@
         <v>323</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -4660,45 +4697,45 @@
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>54</v>
       </c>
       <c r="I14" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
@@ -4707,7 +4744,7 @@
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>114</v>
       </c>
@@ -4721,31 +4758,31 @@
         <v>143</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>256</v>
+        <v>54</v>
       </c>
       <c r="I15" s="7">
         <v>2</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>324</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -4754,45 +4791,45 @@
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="I16" s="7">
         <v>2</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
@@ -4801,7 +4838,7 @@
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>115</v>
       </c>
@@ -4815,13 +4852,13 @@
         <v>144</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>67</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>54</v>
@@ -4836,10 +4873,10 @@
         <v>325</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -4848,45 +4885,45 @@
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>54</v>
       </c>
       <c r="I18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>38</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
@@ -4895,28 +4932,46 @@
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+        <v>145</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="7">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>318</v>
+      </c>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
@@ -4924,18 +4979,18 @@
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -4953,18 +5008,18 @@
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -4982,18 +5037,18 @@
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -5011,18 +5066,18 @@
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -5040,18 +5095,18 @@
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -5069,18 +5124,18 @@
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -5098,18 +5153,18 @@
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -5127,18 +5182,18 @@
       <c r="R26" s="7"/>
       <c r="S26" s="7"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -5156,18 +5211,18 @@
       <c r="R27" s="7"/>
       <c r="S27" s="7"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -5185,18 +5240,18 @@
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>88</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -5214,18 +5269,18 @@
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>88</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -5243,18 +5298,18 @@
       <c r="R30" s="7"/>
       <c r="S30" s="7"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -5272,18 +5327,18 @@
       <c r="R31" s="7"/>
       <c r="S31" s="7"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -5301,18 +5356,18 @@
       <c r="R32" s="7"/>
       <c r="S32" s="7"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -5330,18 +5385,18 @@
       <c r="R33" s="7"/>
       <c r="S33" s="7"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -5359,9 +5414,9 @@
       <c r="R34" s="7"/>
       <c r="S34" s="7"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>99</v>
@@ -5370,7 +5425,7 @@
         <v>100</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -5388,18 +5443,18 @@
       <c r="R35" s="7"/>
       <c r="S35" s="7"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -5417,18 +5472,18 @@
       <c r="R36" s="7"/>
       <c r="S36" s="7"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -5446,9 +5501,9 @@
       <c r="R37" s="7"/>
       <c r="S37" s="7"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>99</v>
@@ -5457,7 +5512,7 @@
         <v>104</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -5475,18 +5530,18 @@
       <c r="R38" s="7"/>
       <c r="S38" s="7"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -5504,8 +5559,34 @@
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
       <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K41" s="7"/>
@@ -5530,6 +5611,9 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>